<commit_message>
planning update blauw gemaakt
</commit_message>
<xml_diff>
--- a/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
+++ b/Concept/Documentation/Groep Alieke - Hanzaki Assetlist & Planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingo\Documents\school\DesignProcess\Gamelab 1 Jaar 2\Concept\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenj2\Documents\Gamelab1-Jaar2\Concept\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1815,7 +1815,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -1939,7 +1939,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1963,12 +1963,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1989,9 +1989,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2029,7 +2029,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2101,7 +2101,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2259,15 +2259,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.75" customWidth="1"/>
-    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" customWidth="1"/>
-    <col min="4" max="4" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.25" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="16.125" customWidth="1"/>
-    <col min="88" max="88" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" customWidth="1"/>
+    <col min="88" max="88" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:151" x14ac:dyDescent="0.25">
@@ -4283,14 +4283,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -9954,32 +9954,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.625" customWidth="1"/>
-    <col min="2" max="2" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.375" customWidth="1"/>
-    <col min="4" max="4" width="3.25" style="14" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="14" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="14" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.375" style="14" customWidth="1"/>
-    <col min="11" max="12" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.75" style="14" customWidth="1"/>
-    <col min="14" max="15" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" style="14" customWidth="1"/>
+    <col min="11" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" style="14" customWidth="1"/>
+    <col min="14" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4" style="14" customWidth="1"/>
-    <col min="17" max="18" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="4" style="14" customWidth="1"/>
-    <col min="20" max="21" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="4" style="14" customWidth="1"/>
-    <col min="23" max="24" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.25" style="14" customWidth="1"/>
+    <col min="23" max="24" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.28515625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -10983,10 +10983,10 @@
       <c r="A55" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="8" t="s">
+      <c r="B55" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="9" t="s">
         <v>131</v>
       </c>
       <c r="D55" s="14"/>
@@ -11014,10 +11014,10 @@
       <c r="A56" s="9" t="s">
         <v>563</v>
       </c>
-      <c r="B56" s="8" t="s">
+      <c r="B56" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="9" t="s">
         <v>133</v>
       </c>
       <c r="D56" s="14"/>
@@ -11040,10 +11040,10 @@
     </row>
     <row r="57" spans="1:25" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="8" t="s">
+      <c r="B57" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="9" t="s">
         <v>134</v>
       </c>
       <c r="D57" s="14"/>
@@ -11071,7 +11071,7 @@
         <v>199</v>
       </c>
       <c r="G58" s="14"/>
-      <c r="I58" s="8" t="s">
+      <c r="I58" s="9" t="s">
         <v>287</v>
       </c>
       <c r="J58" s="14"/>
@@ -11088,7 +11088,7 @@
         <v>201</v>
       </c>
       <c r="G59" s="14"/>
-      <c r="I59" s="8" t="s">
+      <c r="I59" s="9" t="s">
         <v>288</v>
       </c>
       <c r="J59" s="14"/>
@@ -11105,7 +11105,7 @@
         <v>202</v>
       </c>
       <c r="G60" s="14"/>
-      <c r="I60" s="8" t="s">
+      <c r="I60" s="9" t="s">
         <v>289</v>
       </c>
       <c r="J60" s="14"/>
@@ -11119,6 +11119,7 @@
       <c r="A61" s="7"/>
       <c r="D61" s="14"/>
       <c r="G61" s="14"/>
+      <c r="I61" s="9"/>
       <c r="J61" s="14"/>
       <c r="M61" s="14"/>
       <c r="P61" s="14"/>

</xml_diff>